<commit_message>
fixed names once again :dog:
</commit_message>
<xml_diff>
--- a/Python ETL/BASE_DADOS-RH-1.0.xlsx
+++ b/Python ETL/BASE_DADOS-RH-1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolineamarante/Documents/gerenciamento-de-salas-V0.1/Python ETL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696EE40C-282A-684D-869F-E0B47C614B90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FE9DDD-456A-7F4C-A689-E8BBA072FAA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15040" firstSheet="3" activeTab="6" xr2:uid="{DE615C08-F97B-4A36-9702-3D0A64471026}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15040" firstSheet="3" activeTab="5" xr2:uid="{DE615C08-F97B-4A36-9702-3D0A64471026}"/>
   </bookViews>
   <sheets>
     <sheet name="1_SEMESTRE" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="196">
   <si>
     <t>ID</t>
   </si>
@@ -383,12 +383,6 @@
   </si>
   <si>
     <t>Espanhol I</t>
-  </si>
-  <si>
-    <t>Planejamento Estratétigico em Recursos Humanos</t>
-  </si>
-  <si>
-    <t>Coachinhg e Consultoria em Gestão de Recursos Humanos</t>
   </si>
   <si>
     <t>Auditoria e Qualidade em Gestão de Pessoas</t>
@@ -2855,7 +2849,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="142" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F1" s="142"/>
       <c r="G1" s="142"/>
@@ -2955,35 +2949,35 @@
         <v>2</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E4" s="2">
         <f>VLOOKUP(F4,Tabela3[#All],2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G4" s="2">
         <f>VLOOKUP(H4,Tabela3[#All],2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I4" s="2">
         <f>VLOOKUP(J4,Tabela3[#All],2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K4" s="2">
         <f>VLOOKUP(L4,Tabela3[#All],2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="34">
@@ -3037,35 +3031,35 @@
         <v>2</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E6" s="2">
         <f>VLOOKUP(F6,Tabela3[#All],2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G6" s="2">
         <f>VLOOKUP(H6,Tabela3[#All],2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I6" s="2">
         <f>VLOOKUP(J6,Tabela3[#All],2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K6" s="2">
         <f>VLOOKUP(L6,Tabela3[#All],2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:12" hidden="1">
@@ -3135,35 +3129,35 @@
         <v>2</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E9" s="2">
         <f>VLOOKUP(F9,Tabela3[#All],2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G9" s="2">
         <f>VLOOKUP(H9,Tabela3[#All],2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I9" s="2">
         <f>VLOOKUP(J9,Tabela3[#All],2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K9" s="2">
         <f>VLOOKUP(L9,Tabela3[#All],2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="51">
@@ -3217,35 +3211,35 @@
         <v>3</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E11" s="2">
         <f>VLOOKUP(F11,Tabela3[#All],2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G11" s="2">
         <f>VLOOKUP(H11,Tabela3[#All],2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I11" s="2">
         <f>VLOOKUP(J11,Tabela3[#All],2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K11" s="2">
         <f>VLOOKUP(L11,Tabela3[#All],2,FALSE)</f>
         <v>5</v>
       </c>
       <c r="L11" s="24" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="51">
@@ -3299,7 +3293,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E13" s="23">
         <f>VLOOKUP(F13,Tabela3[#All],2,FALSE)</f>
@@ -3313,21 +3307,21 @@
         <v>2</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I13" s="42">
         <f>VLOOKUP(J13,Tabela3[#All],2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K13" s="42">
         <f>VLOOKUP(L13,Tabela3[#All],2,FALSE)</f>
         <v>5</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="14" customHeight="1"/>
@@ -3418,7 +3412,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="142" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F1" s="142"/>
       <c r="G1" s="142"/>
@@ -3518,28 +3512,28 @@
         <v>3</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E4" s="2">
         <f>VLOOKUP(F4,Tabela3[#All],2,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G4" s="2">
         <f>VLOOKUP(H4,Tabela3[#All],2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I4" s="2">
         <f>VLOOKUP(J4,Tabela3[#All],2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K4" s="2">
         <f>VLOOKUP(L4,Tabela3[#All],2,FALSE)</f>
@@ -3600,35 +3594,35 @@
         <v>3</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E6" s="2">
         <f>VLOOKUP(F6,Tabela3[#All],2,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G6" s="2">
         <f>VLOOKUP(H6,Tabela3[#All],2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I6" s="2">
         <f>VLOOKUP(J6,Tabela3[#All],2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K6" s="2">
         <f>VLOOKUP(L6,Tabela3[#All],2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -3698,35 +3692,35 @@
         <v>9</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E9" s="2">
         <f>VLOOKUP(F9,Tabela3[#All],2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G9" s="2">
         <f>VLOOKUP(H9,Tabela3[#All],2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I9" s="2">
         <f>VLOOKUP(J9,Tabela3[#All],2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K9" s="2">
         <f>VLOOKUP(L9,Tabela3[#All],2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="68">
@@ -3780,35 +3774,35 @@
         <v>2</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E11" s="2">
         <f>VLOOKUP(F11,Tabela3[#All],2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G11" s="2">
         <f>VLOOKUP(H11,Tabela3[#All],2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I11" s="2">
         <f>VLOOKUP(J11,Tabela3[#All],2,FALSE)</f>
         <v>4</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K11" s="2">
         <f>VLOOKUP(L11,Tabela3[#All],2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="L11" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="51">
@@ -3862,35 +3856,35 @@
         <v>2</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E13" s="23">
         <f>VLOOKUP(F13,Tabela3[#All],2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G13" s="23">
         <f>VLOOKUP(H13,Tabela3[#All],2,FALSE)</f>
         <v>9</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I13" s="23">
         <f>VLOOKUP(J13,Tabela3[#All],2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K13" s="23">
         <f>VLOOKUP(L13,Tabela3[#All],2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3973,7 +3967,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="142" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F1" s="142"/>
       <c r="G1" s="142"/>
@@ -4073,28 +4067,28 @@
         <v>12</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E4" s="2">
         <f>VLOOKUP(F4,Tabela3[#All],2,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G4" s="2">
         <f>VLOOKUP(H4,Tabela3[#All],2,FALSE)</f>
         <v>16</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I4" s="2">
         <f>VLOOKUP(J4,Tabela3[#All],2,FALSE)</f>
         <v>15</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K4" s="2">
         <f>VLOOKUP(L4,Tabela3[#All],2,FALSE)</f>
@@ -4155,35 +4149,35 @@
         <v>12</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E6" s="2">
         <f>VLOOKUP(F6,Tabela3[#All],2,FALSE)</f>
         <v>15</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G6" s="2">
         <f>VLOOKUP(H6,Tabela3[#All],2,FALSE)</f>
         <v>16</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I6" s="2">
         <f>VLOOKUP(J6,Tabela3[#All],2,FALSE)</f>
         <v>15</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K6" s="2">
         <f>VLOOKUP(L6,Tabela3[#All],2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -4253,35 +4247,35 @@
         <v>14</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E9" s="2">
         <f>VLOOKUP(F9,Tabela3[#All],2,FALSE)</f>
         <v>12</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G9" s="2">
         <f>VLOOKUP(H9,Tabela3[#All],2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I9" s="2">
         <f>VLOOKUP(J9,Tabela3[#All],2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K9" s="2">
         <f>VLOOKUP(L9,Tabela3[#All],2,FALSE)</f>
         <v>14</v>
       </c>
       <c r="L9" s="133" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="43.5" customHeight="1">
@@ -4335,35 +4329,35 @@
         <v>14</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E11" s="2">
         <f>VLOOKUP(F11,Tabela3[#All],2,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G11" s="2">
         <f>VLOOKUP(H11,Tabela3[#All],2,FALSE)</f>
         <v>17</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I11" s="2">
         <f>VLOOKUP(J11,Tabela3[#All],2,FALSE)</f>
         <v>17</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K11" s="2">
         <f>VLOOKUP(L11,Tabela3[#All],2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="48" customHeight="1">
@@ -4417,35 +4411,35 @@
         <v>12</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E13" s="23">
         <f>VLOOKUP(F13,Tabela3[#All],2,FALSE)</f>
         <v>8</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G13" s="23">
         <f>VLOOKUP(H13,Tabela3[#All],2,FALSE)</f>
         <v>17</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I13" s="23">
         <f>VLOOKUP(J13,Tabela3[#All],2,FALSE)</f>
         <v>17</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K13" s="23">
         <f>VLOOKUP(L13,Tabela3[#All],2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="L13" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4534,7 +4528,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="142" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F1" s="142"/>
       <c r="G1" s="142"/>
@@ -4616,7 +4610,7 @@
         <v>48</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="K3" s="2">
         <f>VLOOKUP(L3,Tabela1[#All],2,FALSE)</f>
@@ -4634,28 +4628,28 @@
         <v>7</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E4" s="2">
         <f>VLOOKUP(F4,Tabela3[#All],2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G4" s="2">
         <f>VLOOKUP(H4,Tabela3[#All],2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I4" s="2">
         <f>VLOOKUP(J4,Tabela3[#All],2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K4" s="2">
         <f>VLOOKUP(L4,Tabela3[#All],2,FALSE)</f>
@@ -4698,7 +4692,7 @@
         <v>48</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="K5" s="2">
         <f>VLOOKUP(L5,Tabela1[#All],2,FALSE)</f>
@@ -4716,35 +4710,35 @@
         <v>7</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E6" s="2">
         <f>VLOOKUP(F6,Tabela3[#All],2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G6" s="2">
         <f>VLOOKUP(H6,Tabela3[#All],2,FALSE)</f>
         <v>7</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I6" s="2">
         <f>VLOOKUP(J6,Tabela3[#All],2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K6" s="2">
         <f>VLOOKUP(L6,Tabela3[#All],2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -4814,35 +4808,35 @@
         <v>12</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E9" s="2">
         <f>VLOOKUP(F9,Tabela3[#All],2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G9" s="2">
         <f>VLOOKUP(H9,Tabela3[#All],2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I9" s="2">
         <f>VLOOKUP(J9,Tabela3[#All],2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K9" s="2">
         <f>VLOOKUP(L9,Tabela3[#All],2,FALSE)</f>
         <v>6</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="51">
@@ -4896,28 +4890,28 @@
         <v>12</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E11" s="2">
         <f>VLOOKUP(F11,Tabela3[#All],2,FALSE)</f>
         <v>18</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G11" s="2">
         <f>VLOOKUP(H11,Tabela3[#All],2,FALSE)</f>
         <v>18</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I11" s="2">
         <f>VLOOKUP(J11,Tabela3[#All],2,FALSE)</f>
         <v>19</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K11" s="2">
         <f>VLOOKUP(L11,Tabela3[#All],2,FALSE)</f>
@@ -4978,28 +4972,28 @@
         <v>13</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E13" s="23">
         <f>VLOOKUP(F13,Tabela3[#All],2,FALSE)</f>
         <v>18</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G13" s="23">
         <f>VLOOKUP(H13,Tabela3[#All],2,FALSE)</f>
         <v>18</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I13" s="23">
         <f>VLOOKUP(J13,Tabela3[#All],2,FALSE)</f>
         <v>19</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K13" s="23">
         <f>VLOOKUP(L13,Tabela3[#All],2,FALSE)</f>
@@ -5094,7 +5088,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="142" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F1" s="142"/>
       <c r="G1" s="142"/>
@@ -5194,35 +5188,35 @@
         <v>21</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E4" s="2">
         <f>VLOOKUP(F4,Tabela3[#All],2,FALSE)</f>
         <v>22</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G4" s="2">
         <f>VLOOKUP(H4,Tabela3[#All],2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I4" s="2">
         <f>VLOOKUP(J4,Tabela3[#All],2,FALSE)</f>
         <v>22</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K4" s="2">
         <f>VLOOKUP(L4,Tabela3[#All],2,FALSE)</f>
         <v>23</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="35.25" customHeight="1">
@@ -5276,35 +5270,35 @@
         <v>21</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E6" s="2">
         <f>VLOOKUP(F6,Tabela3[#All],2,FALSE)</f>
         <v>22</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G6" s="2">
         <f>VLOOKUP(H6,Tabela3[#All],2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I6" s="2">
         <f>VLOOKUP(J6,Tabela3[#All],2,FALSE)</f>
         <v>22</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K6" s="2">
         <f>VLOOKUP(L6,Tabela3[#All],2,FALSE)</f>
         <v>23</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="35.25" customHeight="1">
@@ -5374,35 +5368,35 @@
         <v>21</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E9" s="2">
         <f>VLOOKUP(F9,Tabela3[#All],2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G9" s="2">
         <f>VLOOKUP(H9,Tabela3[#All],2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I9" s="2">
         <f>VLOOKUP(J9,Tabela3[#All],2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K9" s="2">
         <f>VLOOKUP(L9,Tabela3[#All],2,FALSE)</f>
         <v>23</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="35.25" customHeight="1">
@@ -5445,7 +5439,7 @@
         <v>49</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="35.25" customHeight="1">
@@ -5456,35 +5450,35 @@
         <v>21</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E11" s="2">
         <f>VLOOKUP(F11,Tabela3[#All],2,FALSE)</f>
         <v>12</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G11" s="2">
         <f>VLOOKUP(H11,Tabela3[#All],2,FALSE)</f>
         <v>16</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I11" s="2">
         <f>VLOOKUP(J11,Tabela3[#All],2,FALSE)</f>
         <v>11</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K11" s="2">
         <f>VLOOKUP(L11,Tabela3[#All],2,FALSE)</f>
         <v>24</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="35.25" customHeight="1">
@@ -5527,7 +5521,7 @@
         <v>49</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="35.25" customHeight="1">
@@ -5545,28 +5539,28 @@
         <v>12</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G13" s="23">
         <f>VLOOKUP(H13,Tabela3[#All],2,FALSE)</f>
         <v>16</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I13" s="23">
         <f>VLOOKUP(J13,Tabela3[#All],2,FALSE)</f>
         <v>23</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K13" s="23">
         <f>VLOOKUP(L13,Tabela3[#All],2,FALSE)</f>
         <v>24</v>
       </c>
       <c r="L13" s="25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -5628,8 +5622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26E5941-C56D-4424-AA01-455D5DE9BA8B}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="15"/>
@@ -5653,7 +5647,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="142" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F1" s="142"/>
       <c r="G1" s="142"/>
@@ -5709,33 +5703,33 @@
       <c r="B3" s="135">
         <v>0.32291666666666669</v>
       </c>
-      <c r="C3" s="2" t="e">
+      <c r="C3" s="2">
         <f>VLOOKUP(D3,Tabela1[#All],2,FALSE)</f>
-        <v>#N/A</v>
+        <v>43</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>116</v>
+        <v>194</v>
       </c>
       <c r="E3" s="2">
         <f>VLOOKUP(F3,Tabela1[#All],2,FALSE)</f>
         <v>47</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G3" s="2">
         <f>VLOOKUP(H3,Tabela1[#All],2,FALSE)</f>
         <v>45</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I3" s="2">
         <f>VLOOKUP(J3,Tabela1[#All],2,FALSE)</f>
         <v>45</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K3" s="2">
         <f>VLOOKUP(L3,Tabela1[#All],2,FALSE)</f>
@@ -5753,28 +5747,28 @@
         <v>13</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E4" s="2">
         <f>VLOOKUP(F4,Tabela3[#All],2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G4" s="2">
         <f>VLOOKUP(H4,Tabela3[#All],2,FALSE)</f>
         <v>25</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I4" s="2">
         <f>VLOOKUP(J4,Tabela3[#All],2,FALSE)</f>
         <v>25</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K4" s="2">
         <f>VLOOKUP(L4,Tabela3[#All],2,FALSE)</f>
@@ -5791,40 +5785,40 @@
       <c r="B5" s="135">
         <v>0.3576388888888889</v>
       </c>
-      <c r="C5" s="2" t="e">
+      <c r="C5" s="2">
         <f>VLOOKUP(D5,Tabela1[#All],2,FALSE)</f>
-        <v>#N/A</v>
+        <v>43</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>116</v>
+        <v>194</v>
       </c>
       <c r="E5" s="2">
         <f>VLOOKUP(F5,Tabela1[#All],2,FALSE)</f>
         <v>47</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G5" s="2">
         <f>VLOOKUP(H5,Tabela1[#All],2,FALSE)</f>
         <v>45</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I5" s="2">
         <f>VLOOKUP(J5,Tabela1[#All],2,FALSE)</f>
         <v>45</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K5" s="2">
         <f>VLOOKUP(L5,Tabela1[#All],2,FALSE)</f>
         <v>44</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="16">
@@ -5835,35 +5829,35 @@
         <v>13</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E6" s="2">
         <f>VLOOKUP(F6,Tabela3[#All],2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G6" s="2">
         <f>VLOOKUP(H6,Tabela3[#All],2,FALSE)</f>
         <v>25</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I6" s="2">
         <f>VLOOKUP(J6,Tabela3[#All],2,FALSE)</f>
         <v>25</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K6" s="2">
         <f>VLOOKUP(L6,Tabela3[#All],2,FALSE)</f>
         <v>21</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -5889,40 +5883,40 @@
       <c r="B8" s="135">
         <v>0.39930555555555558</v>
       </c>
-      <c r="C8" s="2" t="e">
+      <c r="C8" s="2">
         <f>VLOOKUP(D8,Tabela1[#All],2,FALSE)</f>
-        <v>#N/A</v>
+        <v>43</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>116</v>
+        <v>194</v>
       </c>
       <c r="E8" s="2">
         <f>VLOOKUP(F8,Tabela1[#All],2,FALSE)</f>
         <v>50</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="G8" s="2" t="e">
+        <v>192</v>
+      </c>
+      <c r="G8" s="2">
         <f>VLOOKUP(H8,Tabela1[#All],2,FALSE)</f>
-        <v>#N/A</v>
+        <v>42</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>115</v>
+        <v>195</v>
       </c>
       <c r="I8" s="2">
         <f>VLOOKUP(J8,Tabela1[#All],2,FALSE)</f>
         <v>50</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K8" s="2">
         <f>VLOOKUP(L8,Tabela1[#All],2,FALSE)</f>
         <v>44</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="16">
@@ -5933,35 +5927,35 @@
         <v>13</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E9" s="2">
         <f>VLOOKUP(F9,Tabela3[#All],2,FALSE)</f>
         <v>22</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G9" s="2">
         <f>VLOOKUP(H9,Tabela3[#All],2,FALSE)</f>
         <v>9</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I9" s="2">
         <f>VLOOKUP(J9,Tabela3[#All],2,FALSE)</f>
         <v>22</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K9" s="2">
         <f>VLOOKUP(L9,Tabela3[#All],2,FALSE)</f>
         <v>21</v>
       </c>
       <c r="L9" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="85">
@@ -5971,40 +5965,40 @@
       <c r="B10" s="135">
         <v>0.43402777777777773</v>
       </c>
-      <c r="C10" s="2" t="e">
+      <c r="C10" s="2">
         <f>VLOOKUP(D10,Tabela1[#All],2,FALSE)</f>
-        <v>#N/A</v>
+        <v>43</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E10" s="2" t="e">
+        <v>194</v>
+      </c>
+      <c r="E10" s="2">
         <f>VLOOKUP(F10,Tabela1[#All],2,FALSE)</f>
-        <v>#N/A</v>
+        <v>43</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="G10" s="2" t="e">
+        <v>194</v>
+      </c>
+      <c r="G10" s="2">
         <f>VLOOKUP(H10,Tabela1[#All],2,FALSE)</f>
-        <v>#N/A</v>
+        <v>42</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>115</v>
+        <v>195</v>
       </c>
       <c r="I10" s="2">
         <f>VLOOKUP(J10,Tabela1[#All],2,FALSE)</f>
         <v>50</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K10" s="2">
         <f>VLOOKUP(L10,Tabela1[#All],2,FALSE)</f>
         <v>44</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="16">
@@ -6015,35 +6009,35 @@
         <v>13</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E11" s="2">
         <f>VLOOKUP(F11,Tabela3[#All],2,FALSE)</f>
         <v>13</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G11" s="2">
         <f>VLOOKUP(H11,Tabela3[#All],2,FALSE)</f>
         <v>9</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I11" s="2">
         <f>VLOOKUP(J11,Tabela3[#All],2,FALSE)</f>
         <v>22</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K11" s="2">
         <f>VLOOKUP(L11,Tabela3[#All],2,FALSE)</f>
         <v>21</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="68">
@@ -6053,40 +6047,40 @@
       <c r="B12" s="135">
         <v>0.46875</v>
       </c>
-      <c r="C12" s="2" t="e">
+      <c r="C12" s="2">
         <f>VLOOKUP(D12,Tabela1[#All],2,FALSE)</f>
-        <v>#N/A</v>
+        <v>42</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>115</v>
+        <v>195</v>
       </c>
       <c r="E12" s="2">
         <f>VLOOKUP(F12,Tabela1[#All],2,FALSE)</f>
         <v>51</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G12" s="2">
         <f>VLOOKUP(H12,Tabela1[#All],2,FALSE)</f>
         <v>51</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I12" s="2">
         <f>VLOOKUP(J12,Tabela1[#All],2,FALSE)</f>
         <v>50</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K12" s="2">
         <f>VLOOKUP(L12,Tabela1[#All],2,FALSE)</f>
         <v>44</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="17" thickBot="1">
@@ -6097,35 +6091,35 @@
         <v>9</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E13" s="23">
         <f>VLOOKUP(F13,Tabela3[#All],2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G13" s="23">
         <f>VLOOKUP(H13,Tabela3[#All],2,FALSE)</f>
         <v>3</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I13" s="23">
         <f>VLOOKUP(J13,Tabela3[#All],2,FALSE)</f>
         <v>22</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K13" s="23">
         <f>VLOOKUP(L13,Tabela3[#All],2,FALSE)</f>
         <v>21</v>
       </c>
       <c r="L13" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -6169,7 +6163,7 @@
           <x14:formula1>
             <xm:f>Mock_Tables!$B$4:$B$100</xm:f>
           </x14:formula1>
-          <xm:sqref>D3 L3 D12 D10 H3 L10 F10 F12 D8 L8 J3 H5 L12 J5 D5 L5 H12 F3 F5 F8 H8 J12 H10 J8 J10</xm:sqref>
+          <xm:sqref>D3 L3 D12 D8 H3 L10 H10 F12 D5 L8 J3 H5 L12 J5 J10 L5 H12 F3 F5 F8 F10 J12 D10 J8 H8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6B326551-C5CB-46CC-B944-6D9C055C28AA}">
           <x14:formula1>
@@ -6187,8 +6181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF6508E-B8F4-43C4-AACB-99409B526617}">
   <dimension ref="B1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -6334,7 +6328,7 @@
       </c>
       <c r="O4" s="12"/>
       <c r="P4" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="Q4" s="17">
         <v>1</v>
@@ -6356,17 +6350,17 @@
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="78" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F5" s="15">
         <f t="shared" ref="F5:F28" si="1">ROW() - 3</f>
         <v>2</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H5" s="125" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I5" s="13">
         <v>5</v>
@@ -6386,7 +6380,7 @@
       </c>
       <c r="O5" s="12"/>
       <c r="P5" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="Q5" s="17">
         <v>2</v>
@@ -6408,17 +6402,17 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="78" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F6" s="15">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H6" s="125" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I6" s="13">
         <v>5</v>
@@ -6438,7 +6432,7 @@
       </c>
       <c r="O6" s="12"/>
       <c r="P6" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="Q6" s="17">
         <v>3</v>
@@ -6460,17 +6454,17 @@
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="78" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F7" s="15">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H7" s="125" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I7" s="13">
         <v>5</v>
@@ -6490,7 +6484,7 @@
       </c>
       <c r="O7" s="12"/>
       <c r="P7" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="Q7" s="17">
         <v>4</v>
@@ -6512,17 +6506,17 @@
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="78" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F8" s="15">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H8" s="125" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I8" s="13">
         <v>5</v>
@@ -6542,7 +6536,7 @@
       </c>
       <c r="O8" s="12"/>
       <c r="P8" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="Q8" s="17">
         <v>5</v>
@@ -6564,17 +6558,17 @@
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="78" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F9" s="15">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H9" s="125" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I9" s="13">
         <v>5</v>
@@ -6594,7 +6588,7 @@
       </c>
       <c r="O9" s="12"/>
       <c r="P9" s="16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="Q9" s="17">
         <v>6</v>
@@ -6610,17 +6604,17 @@
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="78" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F10" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I10" s="13">
         <v>5</v>
@@ -6651,17 +6645,17 @@
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="73" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F11" s="15">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H11" s="125" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I11" s="13">
         <v>5</v>
@@ -6692,17 +6686,17 @@
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="78" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F12" s="15">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="G12" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="H12" s="125" t="s">
         <v>141</v>
-      </c>
-      <c r="H12" s="125" t="s">
-        <v>143</v>
       </c>
       <c r="I12" s="13">
         <v>5</v>
@@ -6733,17 +6727,17 @@
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="78" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F13" s="15">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H13" s="125" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I13" s="13">
         <v>5</v>
@@ -6774,7 +6768,7 @@
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="78" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F14" s="15">
         <f t="shared" si="1"/>
@@ -6784,7 +6778,7 @@
         <v>64</v>
       </c>
       <c r="H14" s="124" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I14" s="13">
         <v>5</v>
@@ -6815,17 +6809,17 @@
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="78" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F15" s="15">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H15" s="125" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I15" s="13">
         <v>5</v>
@@ -6856,17 +6850,17 @@
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="78" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F16" s="15">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H16" s="125" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I16" s="13">
         <v>5</v>
@@ -6897,7 +6891,7 @@
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="78" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F17" s="15">
         <f t="shared" si="1"/>
@@ -6907,7 +6901,7 @@
         <v>64</v>
       </c>
       <c r="H17" s="125" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I17" s="13">
         <v>5</v>
@@ -6938,17 +6932,17 @@
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="73" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F18" s="15">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H18" s="125" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I18" s="13">
         <v>5</v>
@@ -6979,17 +6973,17 @@
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="78" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F19" s="15">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H19" s="125" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I19" s="13">
         <v>5</v>
@@ -7020,17 +7014,17 @@
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="73" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F20" s="15">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H20" s="125" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I20" s="13">
         <v>5</v>
@@ -7061,17 +7055,17 @@
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="78" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F21" s="15">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H21" s="125" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I21" s="13">
         <v>5</v>
@@ -7102,17 +7096,17 @@
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="73" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F22" s="15">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I22" s="13"/>
       <c r="J22" s="12"/>
@@ -7180,17 +7174,17 @@
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="73" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F24" s="15">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H24" s="125" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I24" s="13"/>
       <c r="J24" s="12"/>
@@ -7219,17 +7213,17 @@
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="73" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F25" s="15">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I25" s="13"/>
       <c r="J25" s="12"/>
@@ -7258,7 +7252,7 @@
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="73" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F26" s="15">
         <f t="shared" si="1"/>
@@ -7268,7 +7262,7 @@
         <v>64</v>
       </c>
       <c r="H26" s="123" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="12"/>
@@ -7297,7 +7291,7 @@
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="73" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F27" s="15">
         <f t="shared" si="1"/>
@@ -7307,7 +7301,7 @@
         <v>64</v>
       </c>
       <c r="H27" s="123" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I27" s="13"/>
       <c r="J27" s="12"/>
@@ -7336,17 +7330,17 @@
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="73" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F28" s="15">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H28" s="125" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I28" s="13"/>
       <c r="J28" s="12"/>
@@ -7663,7 +7657,7 @@
     </row>
     <row r="45" spans="2:14" ht="15" customHeight="1">
       <c r="B45" s="76" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C45" s="17">
         <f t="shared" si="0"/>
@@ -7679,7 +7673,7 @@
     </row>
     <row r="46" spans="2:14" ht="15" customHeight="1">
       <c r="B46" s="76" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C46" s="17">
         <f t="shared" si="0"/>
@@ -7695,7 +7689,7 @@
     </row>
     <row r="47" spans="2:14" ht="15" customHeight="1">
       <c r="B47" s="76" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C47" s="17">
         <f t="shared" si="0"/>
@@ -7711,7 +7705,7 @@
     </row>
     <row r="48" spans="2:14" ht="15" customHeight="1" thickBot="1">
       <c r="B48" s="76" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C48" s="17">
         <f t="shared" si="0"/>
@@ -7729,7 +7723,7 @@
     </row>
     <row r="49" spans="2:3" ht="15" customHeight="1">
       <c r="B49" s="129" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C49" s="17">
         <f t="shared" ref="C49:C54" si="2">ROW() - 3</f>
@@ -7738,7 +7732,7 @@
     </row>
     <row r="50" spans="2:3" ht="15" customHeight="1" thickBot="1">
       <c r="B50" s="130" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C50" s="18">
         <f t="shared" si="2"/>
@@ -7747,7 +7741,7 @@
     </row>
     <row r="51" spans="2:3" ht="15" customHeight="1">
       <c r="B51" s="126" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C51" s="15">
         <f t="shared" si="2"/>
@@ -7756,7 +7750,7 @@
     </row>
     <row r="52" spans="2:3" ht="15" customHeight="1">
       <c r="B52" s="126" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C52" s="15">
         <f t="shared" si="2"/>
@@ -7765,7 +7759,7 @@
     </row>
     <row r="53" spans="2:3" ht="15" customHeight="1">
       <c r="B53" s="126" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C53" s="15">
         <f t="shared" si="2"/>
@@ -7774,7 +7768,7 @@
     </row>
     <row r="54" spans="2:3" ht="15" customHeight="1">
       <c r="B54" s="129" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C54" s="15">
         <f t="shared" si="2"/>
@@ -12811,9 +12805,9 @@
         <f>'6_SEMESTRE'!C4</f>
         <v>13</v>
       </c>
-      <c r="G128" s="115" t="e">
+      <c r="G128" s="115">
         <f>'6_SEMESTRE'!C3</f>
-        <v>#N/A</v>
+        <v>43</v>
       </c>
       <c r="H128" s="116">
         <v>6</v>
@@ -12850,9 +12844,9 @@
         <f>'6_SEMESTRE'!C6</f>
         <v>13</v>
       </c>
-      <c r="G129" s="44" t="e">
+      <c r="G129" s="44">
         <f>'6_SEMESTRE'!C5</f>
-        <v>#N/A</v>
+        <v>43</v>
       </c>
       <c r="H129" s="44">
         <v>6</v>
@@ -12889,9 +12883,9 @@
         <f>'6_SEMESTRE'!C9</f>
         <v>13</v>
       </c>
-      <c r="G130" s="44" t="e">
+      <c r="G130" s="44">
         <f>'6_SEMESTRE'!C8</f>
-        <v>#N/A</v>
+        <v>43</v>
       </c>
       <c r="H130" s="44">
         <v>6</v>
@@ -12928,9 +12922,9 @@
         <f>'6_SEMESTRE'!C11</f>
         <v>13</v>
       </c>
-      <c r="G131" s="44" t="e">
+      <c r="G131" s="44">
         <f>'6_SEMESTRE'!C10</f>
-        <v>#N/A</v>
+        <v>43</v>
       </c>
       <c r="H131" s="44">
         <v>6</v>
@@ -12967,9 +12961,9 @@
         <f>'6_SEMESTRE'!C13</f>
         <v>9</v>
       </c>
-      <c r="G132" s="44" t="e">
+      <c r="G132" s="44">
         <f>'6_SEMESTRE'!C12</f>
-        <v>#N/A</v>
+        <v>42</v>
       </c>
       <c r="H132" s="44">
         <v>6</v>
@@ -13123,9 +13117,9 @@
         <f>'6_SEMESTRE'!E11</f>
         <v>13</v>
       </c>
-      <c r="G136" s="44" t="e">
+      <c r="G136" s="44">
         <f>'6_SEMESTRE'!E10</f>
-        <v>#N/A</v>
+        <v>43</v>
       </c>
       <c r="H136" s="44">
         <v>6</v>
@@ -13279,9 +13273,9 @@
         <f>'6_SEMESTRE'!G9</f>
         <v>9</v>
       </c>
-      <c r="G140" s="43" t="e">
+      <c r="G140" s="43">
         <f>'6_SEMESTRE'!G8</f>
-        <v>#N/A</v>
+        <v>42</v>
       </c>
       <c r="H140" s="44">
         <v>6</v>
@@ -13318,9 +13312,9 @@
         <f>'6_SEMESTRE'!G11</f>
         <v>9</v>
       </c>
-      <c r="G141" s="43" t="e">
+      <c r="G141" s="43">
         <f>'6_SEMESTRE'!G10</f>
-        <v>#N/A</v>
+        <v>42</v>
       </c>
       <c r="H141" s="44">
         <v>6</v>

</xml_diff>